<commit_message>
Changed Final CRMS Deployed in 9
</commit_message>
<xml_diff>
--- a/JBL-CRMS_ALL_DEV/Complete_BOM_JBL-CRMS.xlsx
+++ b/JBL-CRMS_ALL_DEV/Complete_BOM_JBL-CRMS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="186">
   <si>
     <t>HELPTEXT.MENU</t>
   </si>
@@ -361,6 +361,9 @@
     <t>GB.JBL.BA.ATM.CARD.CHG.CHK</t>
   </si>
   <si>
+    <t>JBL.COS.ATM.CARD.MGT.NAU.HD</t>
+  </si>
+  <si>
     <t>JBL.ENQ.CARD.CLOSE.LIST.BR</t>
   </si>
   <si>
@@ -535,6 +538,9 @@
     <t>JBL.ENQ.ATM.USER.LIST.HO</t>
   </si>
   <si>
+    <t>GB.JBL.I.CARD.ISS.VLD</t>
+  </si>
+  <si>
     <t>JBL.ENQ.ATM.APPROVED.LIST.HO</t>
   </si>
   <si>
@@ -566,9 +572,6 @@
   </si>
   <si>
     <t>EB.JBL.CARD.BATCH.INFO.CHECKID</t>
-  </si>
-  <si>
-    <t>GB.JBL.I.CARD.ISS.VLD</t>
   </si>
   <si>
     <t>&gt;</t>
@@ -1337,258 +1340,263 @@
       <c r="H11" s="5" t="s">
         <v>110</v>
       </c>
+      <c r="J11" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="K11" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12">
       <c r="E12" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
       <c r="E13" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
       <c r="E14" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15">
       <c r="E15" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>74</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16">
       <c r="E16" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>65</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17">
       <c r="E17" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18">
       <c r="E18" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19">
       <c r="E19" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20">
       <c r="E20" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21">
       <c r="E21" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22">
       <c r="E22" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23">
       <c r="E23" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24">
       <c r="E24" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25">
       <c r="E25" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26">
       <c r="E26" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27">
       <c r="E27" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28">
       <c r="H28" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29">
-      <c r="H29" s="5"/>
+      <c r="H29" s="8" t="s">
+        <v>170</v>
+      </c>
       <c r="K29" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30">
       <c r="K30" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31">
       <c r="K31" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32">
       <c r="K32" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33">
       <c r="K33" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34">
       <c r="K34" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35">
       <c r="K35" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1613,7 +1621,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -1624,7 +1632,7 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>104</v>
@@ -1635,29 +1643,29 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6">
@@ -1667,7 +1675,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
@@ -1701,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>20</v>
@@ -1716,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>35</v>
@@ -1731,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>48</v>
@@ -1746,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>59</v>
@@ -1761,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>68</v>
@@ -1776,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>77</v>
@@ -1791,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>86</v>
@@ -1806,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1821,7 +1829,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>36</v>
@@ -1836,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>49</v>
@@ -1851,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>60</v>
@@ -1866,7 +1874,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>69</v>
@@ -1881,10 +1889,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D13" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1896,7 +1904,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>23</v>
@@ -1911,7 +1919,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>37</v>
@@ -1926,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>50</v>
@@ -1941,7 +1949,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>61</v>
@@ -1956,7 +1964,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
@@ -1971,7 +1979,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>38</v>
@@ -1986,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>51</v>
@@ -2001,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>62</v>
@@ -2016,7 +2024,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>70</v>
@@ -2031,7 +2039,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>80</v>
@@ -2046,7 +2054,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>87</v>
@@ -2061,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>94</v>
@@ -2076,7 +2084,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>101</v>
@@ -2091,7 +2099,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>107</v>
@@ -2106,10 +2114,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D28" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2121,10 +2129,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D29" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2136,10 +2144,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D30" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2151,10 +2159,10 @@
         <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D31" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2166,10 +2174,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D32" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2181,10 +2189,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D33" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2196,10 +2204,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D34" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2211,10 +2219,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D35" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2226,10 +2234,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D36" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2241,10 +2249,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D37" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2256,10 +2264,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D38" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2271,10 +2279,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D39" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2286,10 +2294,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D40" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2301,10 +2309,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D41" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2316,10 +2324,10 @@
         <v>4</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D42" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2331,10 +2339,10 @@
         <v>4</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D43" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2346,7 +2354,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>25</v>
@@ -2361,7 +2369,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>39</v>
@@ -2376,7 +2384,7 @@
         <v>5</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>52</v>
@@ -2391,7 +2399,7 @@
         <v>5</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>63</v>
@@ -2406,7 +2414,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>71</v>
@@ -2421,7 +2429,7 @@
         <v>5</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>81</v>
@@ -2436,7 +2444,7 @@
         <v>5</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>88</v>
@@ -2451,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>95</v>
@@ -2466,7 +2474,7 @@
         <v>5</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>102</v>
@@ -2481,7 +2489,7 @@
         <v>5</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>108</v>
@@ -2496,7 +2504,7 @@
         <v>6</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>26</v>
@@ -2511,7 +2519,7 @@
         <v>6</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>40</v>
@@ -2526,7 +2534,7 @@
         <v>6</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>53</v>
@@ -2541,7 +2549,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>64</v>
@@ -2556,7 +2564,7 @@
         <v>6</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>72</v>
@@ -2571,7 +2579,7 @@
         <v>6</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>82</v>
@@ -2586,7 +2594,7 @@
         <v>6</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>89</v>
@@ -2601,7 +2609,7 @@
         <v>6</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>96</v>
@@ -2616,7 +2624,7 @@
         <v>6</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>103</v>
@@ -2631,7 +2639,7 @@
         <v>6</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>109</v>
@@ -2646,10 +2654,10 @@
         <v>6</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D64" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2661,10 +2669,10 @@
         <v>6</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D65" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2676,10 +2684,10 @@
         <v>6</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D66" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2691,10 +2699,10 @@
         <v>6</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D67" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2706,10 +2714,10 @@
         <v>6</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D68" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2721,10 +2729,10 @@
         <v>6</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D69" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2736,10 +2744,10 @@
         <v>6</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D70" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2751,10 +2759,10 @@
         <v>6</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D71" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2766,10 +2774,10 @@
         <v>7</v>
       </c>
       <c r="B72" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="D72" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2781,7 +2789,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>73</v>
@@ -2796,7 +2804,7 @@
         <v>7</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>83</v>
@@ -2811,7 +2819,7 @@
         <v>7</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>90</v>
@@ -2826,7 +2834,7 @@
         <v>7</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>97</v>
@@ -2841,7 +2849,7 @@
         <v>7</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>104</v>
@@ -2856,7 +2864,7 @@
         <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>110</v>
@@ -2871,10 +2879,10 @@
         <v>7</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D79" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2886,10 +2894,10 @@
         <v>7</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D80" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2901,10 +2909,10 @@
         <v>7</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D81" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2916,7 +2924,7 @@
         <v>7</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>74</v>
@@ -2931,10 +2939,10 @@
         <v>7</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D83" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2946,10 +2954,10 @@
         <v>7</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D84" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2961,10 +2969,10 @@
         <v>7</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D85" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2976,10 +2984,10 @@
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D86" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2991,10 +2999,10 @@
         <v>7</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D87" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3006,10 +3014,10 @@
         <v>7</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D88" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3021,10 +3029,10 @@
         <v>7</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D89" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3036,10 +3044,10 @@
         <v>7</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D90" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3051,10 +3059,10 @@
         <v>7</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D91" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3066,10 +3074,10 @@
         <v>7</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D92" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3081,10 +3089,10 @@
         <v>7</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D93" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3096,10 +3104,10 @@
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D94" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3111,10 +3119,10 @@
         <v>7</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D95" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3126,10 +3134,10 @@
         <v>8</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D96" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3141,10 +3149,10 @@
         <v>8</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D97" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3156,10 +3164,10 @@
         <v>8</v>
       </c>
       <c r="B98" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C98" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="D98" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3171,10 +3179,10 @@
         <v>8</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D99" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3186,7 +3194,7 @@
         <v>8</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>74</v>
@@ -3201,7 +3209,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>28</v>
@@ -3216,7 +3224,7 @@
         <v>9</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>43</v>
@@ -3231,7 +3239,7 @@
         <v>9</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>55</v>
@@ -3246,7 +3254,7 @@
         <v>9</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>66</v>
@@ -3261,7 +3269,7 @@
         <v>9</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>75</v>
@@ -3276,7 +3284,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>84</v>
@@ -3291,7 +3299,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>91</v>
@@ -3306,7 +3314,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>98</v>
@@ -3321,7 +3329,7 @@
         <v>9</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>105</v>
@@ -3336,7 +3344,7 @@
         <v>10</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>29</v>
@@ -3351,7 +3359,7 @@
         <v>10</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>44</v>
@@ -3366,7 +3374,7 @@
         <v>10</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>56</v>
@@ -3381,7 +3389,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>67</v>
@@ -3396,7 +3404,7 @@
         <v>10</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>76</v>
@@ -3411,7 +3419,7 @@
         <v>10</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>85</v>
@@ -3426,7 +3434,7 @@
         <v>10</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>92</v>
@@ -3441,7 +3449,7 @@
         <v>10</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>99</v>
@@ -3456,7 +3464,7 @@
         <v>10</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>106</v>
@@ -3471,10 +3479,10 @@
         <v>10</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D119" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3486,10 +3494,10 @@
         <v>10</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D120" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3501,10 +3509,10 @@
         <v>10</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D121" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3516,10 +3524,10 @@
         <v>10</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D122" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3531,10 +3539,10 @@
         <v>10</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D123" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3546,10 +3554,10 @@
         <v>10</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D124" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3561,10 +3569,10 @@
         <v>10</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D125" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3576,10 +3584,10 @@
         <v>10</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D126" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3591,10 +3599,10 @@
         <v>10</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D127" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3606,10 +3614,10 @@
         <v>10</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D128" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3621,10 +3629,10 @@
         <v>10</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D129" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3636,10 +3644,10 @@
         <v>10</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D130" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3651,10 +3659,10 @@
         <v>10</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D131" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3666,10 +3674,10 @@
         <v>10</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D132" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3681,10 +3689,10 @@
         <v>10</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D133" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3696,10 +3704,10 @@
         <v>10</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D134" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3711,10 +3719,10 @@
         <v>10</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D135" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3726,10 +3734,10 @@
         <v>10</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D136" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3741,10 +3749,10 @@
         <v>10</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D137" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3756,10 +3764,10 @@
         <v>10</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D138" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3771,10 +3779,10 @@
         <v>10</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D139" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3786,10 +3794,10 @@
         <v>10</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D140" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3801,10 +3809,10 @@
         <v>10</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D141" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3816,10 +3824,10 @@
         <v>10</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D142" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3831,10 +3839,10 @@
         <v>10</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D143" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3846,7 +3854,7 @@
         <v>11</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>30</v>
@@ -3861,7 +3869,7 @@
         <v>11</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>45</v>
@@ -3876,7 +3884,7 @@
         <v>11</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>57</v>
@@ -3891,7 +3899,7 @@
         <v>11</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>45</v>
@@ -3906,7 +3914,7 @@
         <v>11</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>30</v>
@@ -3921,7 +3929,7 @@
         <v>11</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C149" s="5" t="s">
         <v>57</v>
@@ -3936,7 +3944,7 @@
         <v>11</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C150" s="5" t="s">
         <v>93</v>
@@ -3951,7 +3959,7 @@
         <v>11</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C151" s="5" t="s">
         <v>100</v>
@@ -3966,10 +3974,10 @@
         <v>13</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D152" s="9" t="str">
         <f t="shared" si="1"/>
@@ -3981,7 +3989,7 @@
         <v>14</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C153" s="5" t="s">
         <v>21</v>
@@ -3996,7 +4004,7 @@
         <v>15</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>33</v>
@@ -4011,7 +4019,7 @@
         <v>16</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C155" s="10">
         <v>17211.0</v>
@@ -4026,7 +4034,7 @@
         <v>16</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C156" s="10">
         <v>52048.0</v>
@@ -4041,7 +4049,7 @@
         <v>16</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C157" s="10">
         <v>52047.0</v>
@@ -4056,7 +4064,7 @@
         <v>16</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C158" s="10">
         <v>17208.0</v>
@@ -4071,7 +4079,7 @@
         <v>16</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C159" s="10">
         <v>17257.0</v>
@@ -4086,7 +4094,7 @@
         <v>17</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C160" s="10">
         <v>399.0</v>
@@ -4101,7 +4109,7 @@
         <v>17</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C161" s="10">
         <v>546.0</v>
@@ -4116,7 +4124,7 @@
         <v>17</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C162" s="10">
         <v>547.0</v>
@@ -4131,7 +4139,7 @@
         <v>18</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C163" s="5" t="s">
         <v>34</v>
@@ -4146,7 +4154,7 @@
         <v>18</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>47</v>
@@ -4161,7 +4169,7 @@
         <v>18</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>58</v>
@@ -4176,7 +4184,7 @@
         <v>19</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C166" s="10">
         <v>30.20210415</v>
@@ -4191,7 +4199,7 @@
         <v>19</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C167" s="10">
         <v>64.20210415</v>
@@ -4206,7 +4214,7 @@
         <v>7</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>27</v>
@@ -4221,7 +4229,7 @@
         <v>7</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>41</v>
@@ -4236,7 +4244,7 @@
         <v>7</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C172" s="5" t="s">
         <v>42</v>

</xml_diff>